<commit_message>
EDGE species and EDGE countries working
</commit_message>
<xml_diff>
--- a/03_docs/metric_template.xlsx
+++ b/03_docs/metric_template.xlsx
@@ -8,19 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sb42kg\Documents\kew_metrics\03_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FCC61F4A-3EEC-41EE-A848-446D977A0410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD6A8E7-39B4-4CDF-AC7F-0A1F7DE86E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{013B2BC5-4B4D-4D56-BB86-C0A847F40B8F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{013B2BC5-4B4D-4D56-BB86-C0A847F40B8F}"/>
   </bookViews>
   <sheets>
     <sheet name="metric_template" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="123">
   <si>
     <t>data</t>
   </si>
@@ -290,6 +305,105 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Response</t>
+  </si>
+  <si>
+    <t>Pironon dataset ?</t>
+  </si>
+  <si>
+    <t>theme2</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>theme2 order</t>
+  </si>
+  <si>
+    <t>sidebar order</t>
+  </si>
+  <si>
+    <t>NBS examples?</t>
+  </si>
+  <si>
+    <t>Link to GBF goals and indicators</t>
+  </si>
+  <si>
+    <t>Restoration?</t>
+  </si>
+  <si>
+    <t>health check</t>
+  </si>
+  <si>
+    <t>day cost</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>vat</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Red List Plants?</t>
+  </si>
+  <si>
+    <t>not sure we have rights?</t>
+  </si>
+  <si>
+    <t>Risk</t>
+  </si>
+  <si>
+    <t>Ecosystem Red List</t>
+  </si>
+  <si>
+    <t>Case studies?</t>
+  </si>
+  <si>
+    <t>Tarciso, Justin</t>
+  </si>
+  <si>
+    <t>Infraspecific</t>
+  </si>
+  <si>
+    <t>Specific</t>
+  </si>
+  <si>
+    <t>Infrageneric</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>Infrafamilial</t>
+  </si>
+  <si>
+    <t>Familial</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>nom. nov**</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>comb. nov*</t>
+  </si>
+  <si>
+    <t>tax. nov</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Ne examples?</t>
   </si>
 </sst>
 </file>
@@ -438,7 +552,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -616,6 +730,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -779,11 +899,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1159,523 +1292,1475 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08871833-759A-4AB6-B1CE-97BEB5883754}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.1796875" customWidth="1"/>
-    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="47.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="51.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <v>385689</v>
+      </c>
+      <c r="N8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="K14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="K15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+      <c r="K19" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="K20" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="4">
+        <v>4</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G23" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q23" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>68</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
         <v>76</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>68</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>45</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G25" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>68</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
         <v>65</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G26" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="G27" s="8"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2" t="s">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
-      </c>
-      <c r="M8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="M11" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>80</v>
-      </c>
-      <c r="N13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" t="s">
-        <v>20</v>
-      </c>
-      <c r="N16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" t="s">
-        <v>23</v>
-      </c>
-      <c r="N20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J23">
-        <v>385689</v>
-      </c>
-      <c r="K23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J24" s="1">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="1">
         <v>354000</v>
       </c>
-      <c r="K24" t="s">
+      <c r="N28" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="D29" t="s">
+        <v>97</v>
+      </c>
+      <c r="M29">
         <v>345230</v>
       </c>
-      <c r="K25" t="s">
+      <c r="N29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="I28">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="L32">
         <v>0.19071842899999999</v>
       </c>
-      <c r="J28">
+      <c r="M32">
         <v>73558</v>
       </c>
-      <c r="K28" t="s">
+      <c r="N32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="I29">
+    <row r="33" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L33">
         <v>0.20659604500000001</v>
       </c>
-      <c r="J29">
+      <c r="M33">
         <v>73135</v>
       </c>
-      <c r="K29" t="s">
+      <c r="N33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="I30">
+    <row r="34" spans="12:14" x14ac:dyDescent="0.35">
+      <c r="L34">
         <v>0.20639283999999999</v>
       </c>
-      <c r="J30">
+      <c r="M34">
         <v>71253</v>
       </c>
-      <c r="K30" t="s">
+      <c r="N34" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P30">
-    <sortCondition ref="A2:A30"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R34">
+    <sortCondition ref="C2:C34"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E90BDA5-18EB-482C-9860-3922611AE135}">
+  <dimension ref="A3:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3">
+        <v>2000</v>
+      </c>
+      <c r="F3">
+        <f>E3+(E3*0.2)</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>800</v>
+      </c>
+      <c r="E4">
+        <f>D4*C4</f>
+        <v>4800</v>
+      </c>
+      <c r="F4">
+        <f>E4+(D4*0.2)</f>
+        <v>4960</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f>SUM(F3:F4)</f>
+        <v>7360</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1200</v>
+      </c>
+      <c r="C10">
+        <f>B10*0.2</f>
+        <v>240</v>
+      </c>
+      <c r="D10">
+        <f>SUM(B10:C10)</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1200</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C14" si="0">B11*0.2</f>
+        <v>240</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D14" si="1">SUM(B11:C11)</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>1200</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1200</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>1200</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <f>SUM(D10:D14)</f>
+        <v>7200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460E3F88-40B4-461C-A8C0-07A83D8C5EBF}">
+  <dimension ref="B2:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>175</v>
+      </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3">
+        <v>187</v>
+      </c>
+      <c r="J3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4">
+        <v>341</v>
+      </c>
+      <c r="D4">
+        <v>1771</v>
+      </c>
+      <c r="E4">
+        <v>62</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4">
+        <v>2187</v>
+      </c>
+      <c r="J4">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5">
+        <v>145</v>
+      </c>
+      <c r="D5">
+        <v>2044</v>
+      </c>
+      <c r="E5">
+        <v>44</v>
+      </c>
+      <c r="F5">
+        <v>115</v>
+      </c>
+      <c r="G5">
+        <v>85</v>
+      </c>
+      <c r="H5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I5">
+        <v>2433</v>
+      </c>
+      <c r="J5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>214</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6">
+        <v>220</v>
+      </c>
+      <c r="J6">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7">
+        <v>406</v>
+      </c>
+      <c r="D7">
+        <v>2570</v>
+      </c>
+      <c r="E7">
+        <v>68</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7">
+        <v>3060</v>
+      </c>
+      <c r="J7">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8">
+        <v>178</v>
+      </c>
+      <c r="D8">
+        <v>2163</v>
+      </c>
+      <c r="E8">
+        <v>75</v>
+      </c>
+      <c r="F8">
+        <v>113</v>
+      </c>
+      <c r="G8">
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>2561</v>
+      </c>
+      <c r="J8">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>110</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>118</v>
+      </c>
+      <c r="H9" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9">
+        <v>130</v>
+      </c>
+      <c r="J9">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10">
+        <v>433</v>
+      </c>
+      <c r="D10">
+        <v>2161</v>
+      </c>
+      <c r="E10">
+        <v>66</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I10">
+        <v>2668</v>
+      </c>
+      <c r="J10">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11">
+        <v>209</v>
+      </c>
+      <c r="D11">
+        <v>2597</v>
+      </c>
+      <c r="E11">
+        <v>115</v>
+      </c>
+      <c r="F11">
+        <v>106</v>
+      </c>
+      <c r="G11">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11">
+        <v>3062</v>
+      </c>
+      <c r="J11">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>250</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12">
+        <v>266</v>
+      </c>
+      <c r="J12">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13">
+        <v>539</v>
+      </c>
+      <c r="D13">
+        <v>2316</v>
+      </c>
+      <c r="E13">
+        <v>70</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13">
+        <v>2936</v>
+      </c>
+      <c r="J13">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14">
+        <v>196</v>
+      </c>
+      <c r="D14">
+        <v>2465</v>
+      </c>
+      <c r="E14">
+        <v>93</v>
+      </c>
+      <c r="F14">
+        <v>86</v>
+      </c>
+      <c r="G14">
+        <v>29</v>
+      </c>
+      <c r="H14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14">
+        <v>2869</v>
+      </c>
+      <c r="J14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>179</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15">
+        <v>195</v>
+      </c>
+      <c r="J15">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16">
+        <v>599</v>
+      </c>
+      <c r="D16">
+        <v>2467</v>
+      </c>
+      <c r="E16">
+        <v>93</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16">
+        <v>3165</v>
+      </c>
+      <c r="J16">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17">
+        <v>250</v>
+      </c>
+      <c r="D17">
+        <v>2709</v>
+      </c>
+      <c r="E17">
+        <v>123</v>
+      </c>
+      <c r="F17">
+        <v>151</v>
+      </c>
+      <c r="G17">
+        <v>52</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>3286</v>
+      </c>
+      <c r="J17">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>